<commit_message>
Fixed "protected sheet" error
</commit_message>
<xml_diff>
--- a/Sharepoint Mailing/Sharepoint Mailing/bin/Debug/ZSOX report template.xlsx
+++ b/Sharepoint Mailing/Sharepoint Mailing/bin/Debug/ZSOX report template.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13200"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz3" sheetId="3" r:id="rId1"/>
-    <sheet name="Arkusz2" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Arkusz1" sheetId="4" r:id="rId2"/>
+    <sheet name="Arkusz2" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId4"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -83,6 +82,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Etykiety wierszy</t>
+  </si>
+  <si>
+    <t>Suma końcowa</t>
+  </si>
+  <si>
+    <t>Etykiety kolumn</t>
+  </si>
+  <si>
+    <t>Suma z Total</t>
   </si>
 </sst>
 </file>
@@ -266,19 +277,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -339,6 +337,21 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -348,7 +361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <protection hidden="1"/>
@@ -380,7 +393,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -389,12 +402,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -403,13 +410,31 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -419,16 +444,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -442,11 +464,344 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+  </extLst>
+</styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Gzik, Leszek" refreshedDate="43518.347500694443" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="10">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A2:P2880" sheet="Arkusz3"/>
+  </cacheSource>
+  <cacheFields count="16">
+    <cacheField name="Date" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="File name (if possible with link to file)" numFmtId="0">
+      <sharedItems containsNonDate="0" containsBlank="1" count="2">
+        <m/>
+        <s v="ZSOX example.xlsb" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="User" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="User Name" numFmtId="0">
+      <sharedItems containsNonDate="0" containsBlank="1" count="2">
+        <m/>
+        <s v="Michał Zieja" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="E-Mail Address" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="File tab" numFmtId="0">
+      <sharedItems containsNonDate="0" containsBlank="1" count="2">
+        <m/>
+        <s v="SM20" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Incident Number" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Comments" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Approver" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Comment" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Key User Approval/Comment" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Approval in incident (Yes/No)" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Stream" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Stream Lead Name" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Stream Lead E-Mail Address" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
     </ext>
   </extLst>
-</styleSheet>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="10">
+  <r>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" showMissing="0" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A4:B6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item sd="0" x="0"/>
+        <item m="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item m="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item m="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="1">
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="1">
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma z Total" fld="12" baseField="5" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="1">
+    <filter fld="1" type="captionNotEqual" evalOrder="-1" id="1" stringValue1="(puste)">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <customFilters>
+            <customFilter operator="notEqual" val="(puste)"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+  </filters>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -748,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,20 +1120,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="21" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="22"/>
-      <c r="P1" s="23"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:18" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -817,7 +1172,7 @@
       <c r="L2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="18" t="s">
         <v>20</v>
       </c>
       <c r="N2" s="11" t="s">
@@ -831,168 +1186,170 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1005,6 +1362,50 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="21">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added back Reminder function
</commit_message>
<xml_diff>
--- a/Sharepoint Mailing/Sharepoint Mailing/bin/Debug/ZSOX report template.xlsx
+++ b/Sharepoint Mailing/Sharepoint Mailing/bin/Debug/ZSOX report template.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="90" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -469,7 +469,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Gzik, Leszek" refreshedDate="43518.347500694443" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="10">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Gzik, Leszek" refreshedDate="43518.347500694443" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="10">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:P2880" sheet="Arkusz3"/>
   </cacheSource>
@@ -726,7 +726,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" showMissing="0" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna1" cacheId="90" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" showMissing="0" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:B6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -1093,7 +1093,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>